<commit_message>
fig dense added, and some other stuff
</commit_message>
<xml_diff>
--- a/02 Deep Learning/02 Evaluation/01 RetinaNet with Angle/02 On Pallet Dataset/OP_Full_SmoothL1_Result_Summary.xlsx
+++ b/02 Deep Learning/02 Evaluation/01 RetinaNet with Angle/02 On Pallet Dataset/OP_Full_SmoothL1_Result_Summary.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mads\Documents\GitHub\BachelorProject\02 Deep Learning\02 Evaluation\01 RetinaNet with Angle\02 On Pallet Dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{340CBABF-DB7B-458F-BE69-96BEFFFB6836}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47330E00-5A5B-47EC-B7AF-5F125B21932B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="368" yWindow="368" windowWidth="13679" windowHeight="9532" xr2:uid="{56D281DB-F793-4E23-A2A1-A969E3E14AA6}"/>
+    <workbookView xWindow="1388" yWindow="2017" windowWidth="13680" windowHeight="9533" xr2:uid="{56D281DB-F793-4E23-A2A1-A969E3E14AA6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Test</t>
   </si>
@@ -69,6 +69,12 @@
   </si>
   <si>
     <t>time</t>
+  </si>
+  <si>
+    <t>time per img</t>
+  </si>
+  <si>
+    <t>center err mm</t>
   </si>
 </sst>
 </file>
@@ -420,10 +426,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86DA3224-ABC6-4198-9CFC-8EEEE3CF292B}">
-  <dimension ref="A1:I14"/>
+  <dimension ref="A1:K14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -431,7 +437,7 @@
     <col min="7" max="7" width="11.19921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -454,13 +460,19 @@
         <v>10</v>
       </c>
       <c r="H1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" t="s">
         <v>9</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="K1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>0</v>
       </c>
@@ -483,13 +495,21 @@
         <v>2.49744907529423</v>
       </c>
       <c r="H2">
+        <f>G2*1670/((914.885+917.224)/2)</f>
+        <v>4.552938668759734</v>
+      </c>
+      <c r="I2">
         <v>2.5267744532469898</v>
       </c>
-      <c r="I2">
+      <c r="J2">
         <v>16.4634810369934</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="K2">
+        <f>J2/99*1000</f>
+        <v>166.29778825245859</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>1</v>
       </c>
@@ -512,13 +532,21 @@
         <v>2.3017043510386799</v>
       </c>
       <c r="H3">
+        <f t="shared" ref="H3:H7" si="0">G3*1670/((914.885+917.224)/2)</f>
+        <v>4.1960890604593892</v>
+      </c>
+      <c r="I3">
         <v>2.1730526120005398</v>
       </c>
-      <c r="I3">
+      <c r="J3">
         <v>16.4235960570076</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="K3">
+        <f t="shared" ref="K3:K7" si="1">J3/99*1000</f>
+        <v>165.89490966674344</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>2</v>
       </c>
@@ -541,13 +569,21 @@
         <v>2.71728943303496</v>
       </c>
       <c r="H4">
+        <f t="shared" si="0"/>
+        <v>4.9537154756276873</v>
+      </c>
+      <c r="I4">
         <v>3.0513560703975902</v>
       </c>
-      <c r="I4">
+      <c r="J4">
         <v>16.5171831509942</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="K4">
+        <f t="shared" si="1"/>
+        <v>166.84023384842624</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>3</v>
       </c>
@@ -570,13 +606,21 @@
         <v>2.6442506862353001</v>
       </c>
       <c r="H5">
+        <f t="shared" si="0"/>
+        <v>4.8205632372451106</v>
+      </c>
+      <c r="I5">
         <v>2.8722049401852998</v>
       </c>
-      <c r="I5">
+      <c r="J5">
         <v>16.631436991003199</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="K5">
+        <f t="shared" si="1"/>
+        <v>167.99431304043637</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>4</v>
       </c>
@@ -599,13 +643,21 @@
         <v>2.6909406568929599</v>
       </c>
       <c r="H6">
+        <f t="shared" si="0"/>
+        <v>4.9056807176988304</v>
+      </c>
+      <c r="I6">
         <v>3.00876886817642</v>
       </c>
-      <c r="I6">
+      <c r="J6">
         <v>16.468287782015899</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="K6">
+        <f t="shared" si="1"/>
+        <v>166.34634123248381</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>5</v>
       </c>
@@ -628,13 +680,21 @@
         <v>2.3904284967388798</v>
       </c>
       <c r="H7">
+        <f t="shared" si="0"/>
+        <v>4.3578363400364601</v>
+      </c>
+      <c r="I7">
         <v>2.3120558699243698</v>
       </c>
-      <c r="I7">
+      <c r="J7">
         <v>16.535083553972001</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="K7">
+        <f t="shared" si="1"/>
+        <v>167.02104599971719</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -643,35 +703,43 @@
         <v>0.90978975518725147</v>
       </c>
       <c r="C8">
-        <f t="shared" ref="C8:D8" si="0">AVERAGE(C2:C7)</f>
+        <f t="shared" ref="C8:D8" si="2">AVERAGE(C2:C7)</f>
         <v>0.8980265053298756</v>
       </c>
       <c r="D8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.90384636695422016</v>
       </c>
       <c r="E8">
-        <f t="shared" ref="E8" si="1">AVERAGE(E2:E7)</f>
+        <f t="shared" ref="E8" si="3">AVERAGE(E2:E7)</f>
         <v>0.92793566172973019</v>
       </c>
       <c r="F8">
-        <f t="shared" ref="F8:H8" si="2">AVERAGE(F2:F7)</f>
+        <f t="shared" ref="F8:H8" si="4">AVERAGE(F2:F7)</f>
         <v>0.70986525444713544</v>
       </c>
       <c r="G8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>2.5403437832058349</v>
       </c>
       <c r="H8">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="H8" si="5">AVERAGE(H2:H7)</f>
+        <v>4.6311372499712018</v>
+      </c>
+      <c r="I8">
+        <f>AVERAGE(I2:I7)</f>
         <v>2.657368802321868</v>
       </c>
-      <c r="I8">
-        <f t="shared" ref="I8" si="3">AVERAGE(I2:I7)</f>
+      <c r="J8">
+        <f t="shared" ref="J8:K8" si="6">AVERAGE(J2:J7)</f>
         <v>16.506511428664385</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="K8">
+        <f t="shared" si="6"/>
+        <v>166.73243867337763</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -680,35 +748,43 @@
         <v>5.7580828668398224E-3</v>
       </c>
       <c r="C9">
-        <f t="shared" ref="C9:F9" si="4">_xlfn.STDEV.S(C2:C7)</f>
+        <f t="shared" ref="C9:F9" si="7">_xlfn.STDEV.S(C2:C7)</f>
         <v>1.4207270614490895E-2</v>
       </c>
       <c r="D9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>9.6682758242879318E-3</v>
       </c>
       <c r="E9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0.12241788021771234</v>
       </c>
       <c r="F9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>8.9505027036373003E-2</v>
       </c>
       <c r="G9">
-        <f t="shared" ref="G9:H9" si="5">_xlfn.STDEV.S(G2:G7)</f>
+        <f t="shared" ref="G9:H9" si="8">_xlfn.STDEV.S(G2:G7)</f>
         <v>0.1709088374094887</v>
       </c>
       <c r="H9">
-        <f t="shared" si="5"/>
+        <f t="shared" ref="H9" si="9">_xlfn.STDEV.S(H2:H7)</f>
+        <v>0.3115729014745805</v>
+      </c>
+      <c r="I9">
+        <f>_xlfn.STDEV.S(I2:I7)</f>
         <v>0.37302027218880401</v>
       </c>
-      <c r="I9">
-        <f t="shared" ref="I9" si="6">_xlfn.STDEV.S(I2:I7)</f>
+      <c r="J9">
+        <f t="shared" ref="J9:K9" si="10">_xlfn.STDEV.S(J2:J7)</f>
         <v>7.3108506694087166E-2</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="K9">
+        <f t="shared" si="10"/>
+        <v>0.73846976458674596</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>6</v>
       </c>

</xml_diff>